<commit_message>
Update ToDo. Added description block
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>done</t>
   </si>
@@ -143,6 +143,99 @@
   </si>
   <si>
     <t>5 m</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Create start window in application with login and password inputs</t>
+  </si>
+  <si>
+    <t>Create main window with setting fields from Performanse Counters and buttons Start and Stop</t>
+  </si>
+  <si>
+    <t>Create model which includes main application work</t>
+  </si>
+  <si>
+    <t>Create subodules "Managers" from control every parts application</t>
+  </si>
+  <si>
+    <t>Add initialization select Performance Counters</t>
+  </si>
+  <si>
+    <t>Add cached files in application</t>
+  </si>
+  <si>
+    <t>Add complex Performance Couters from work with Matworl Loader</t>
+  </si>
+  <si>
+    <t>Add class from work with system processes</t>
+  </si>
+  <si>
+    <t>Create logger from created log files</t>
+  </si>
+  <si>
+    <t>Beatiful display Message Box in logger class</t>
+  </si>
+  <si>
+    <t>Add window from realization function</t>
+  </si>
+  <si>
+    <t>Add hidden main window in Windows start panel</t>
+  </si>
+  <si>
+    <t>Add validation from input fields in main window</t>
+  </si>
+  <si>
+    <t>Create console application from receive messages from the client</t>
+  </si>
+  <si>
+    <t>Connect EnityFramework to application and create database model</t>
+  </si>
+  <si>
+    <t>Add tools from registration user in database</t>
+  </si>
+  <si>
+    <t>Add conditions on main window from separate user logic</t>
+  </si>
+  <si>
+    <t>Add ResourceDictinary from plugins</t>
+  </si>
+  <si>
+    <t>Create new window from check currentsystem data</t>
+  </si>
+  <si>
+    <t>Add checkbox on main window from setting disabling message box</t>
+  </si>
+  <si>
+    <t>Add resx files from localization app</t>
+  </si>
+  <si>
+    <t>Create VisualStudio Installers from Server and Application</t>
+  </si>
+  <si>
+    <t>Added upload current user setting to database</t>
+  </si>
+  <si>
+    <t>Add new folder in AppData from each user. Create uniqle log file from him</t>
+  </si>
+  <si>
+    <t>Create uniqle cach file from each user</t>
+  </si>
+  <si>
+    <t>Create block from check USB device</t>
+  </si>
+  <si>
+    <t>Add Name current user in windows Title</t>
+  </si>
+  <si>
+    <t>Update validation from time fields to 5 seconds</t>
+  </si>
+  <si>
+    <t>Add validation on input field from Process Windows</t>
+  </si>
+  <si>
+    <t>Refactoring code on new branch</t>
   </si>
 </sst>
 </file>
@@ -484,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E31"/>
+  <dimension ref="B1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +593,7 @@
     <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -513,8 +606,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -527,8 +623,11 @@
       <c r="E2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -541,8 +640,11 @@
       <c r="E3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -555,8 +657,11 @@
       <c r="E4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>8</v>
       </c>
@@ -569,8 +674,11 @@
       <c r="E5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -583,8 +691,11 @@
       <c r="E6" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>10</v>
       </c>
@@ -597,8 +708,11 @@
       <c r="E7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -611,8 +725,11 @@
       <c r="E8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -625,8 +742,11 @@
       <c r="E9" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -639,8 +759,11 @@
       <c r="E10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -653,8 +776,11 @@
       <c r="E11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -667,8 +793,11 @@
       <c r="E12" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -681,8 +810,11 @@
       <c r="E13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -695,8 +827,11 @@
       <c r="E14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -709,8 +844,11 @@
       <c r="E15" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -723,8 +861,11 @@
       <c r="E16" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>20</v>
       </c>
@@ -737,8 +878,11 @@
       <c r="E17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>21</v>
       </c>
@@ -751,8 +895,11 @@
       <c r="E18" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>22</v>
       </c>
@@ -765,8 +912,11 @@
       <c r="E19" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>39</v>
       </c>
@@ -779,8 +929,11 @@
       <c r="E20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -793,8 +946,11 @@
       <c r="E21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>24</v>
       </c>
@@ -807,8 +963,11 @@
       <c r="E22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>25</v>
       </c>
@@ -821,8 +980,11 @@
       <c r="E23" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>41</v>
       </c>
@@ -835,8 +997,11 @@
       <c r="E24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -849,8 +1014,11 @@
       <c r="E25" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>27</v>
       </c>
@@ -863,8 +1031,11 @@
       <c r="E26" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>28</v>
       </c>
@@ -877,8 +1048,11 @@
       <c r="E27" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>29</v>
       </c>
@@ -891,8 +1065,11 @@
       <c r="E28" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>30</v>
       </c>
@@ -905,8 +1082,11 @@
       <c r="E29" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>31</v>
       </c>
@@ -919,8 +1099,11 @@
       <c r="E30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>32</v>
       </c>
@@ -932,6 +1115,9 @@
       </c>
       <c r="E31" t="s">
         <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>